<commit_message>
Working version with MVEL
</commit_message>
<xml_diff>
--- a/reconciliation-engine/illustrations/Recon2.0_Template.xlsx
+++ b/reconciliation-engine/illustrations/Recon2.0_Template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saiprasadkrishnamurthy/2.0/recon2.0/reconciliation-engine/illustrations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C80808-6EFA-1F48-ACE2-1577D5C3B1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5697C465-D18A-D94F-9945-BBB8E95461AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{C08B0C19-EF01-7B46-898D-9F2EEE986A3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>Datasource</t>
   </si>
@@ -129,12 +130,6 @@
     <t>tds</t>
   </si>
   <si>
-    <t>TRANSACTION_TOTALS_MATCHED_BETWEEN_SALES_AND_TDSLEDGER</t>
-  </si>
-  <si>
-    <t>TRANSACTION_TOTALS_UNMATCHED_BETWEEN_SALES_AND_TDSLEDGER</t>
-  </si>
-  <si>
     <t>Sub Bucket Fields 1</t>
   </si>
   <si>
@@ -144,27 +139,15 @@
     <t>taxFiled</t>
   </si>
   <si>
-    <t>TRANSACTION_TOTALS_MATCHED_BETWEEN_TDSLEDGER_AND_26AS</t>
-  </si>
-  <si>
-    <t>TRANSACTION_TOTALS_UNMATCHED_BETWEEN_TDSLEDGER_AND_26AS</t>
-  </si>
-  <si>
     <t>TotalsChecks</t>
   </si>
   <si>
-    <t>EntryWiseOneToManyChecks</t>
-  </si>
-  <si>
     <t>ValueWithinToleranceCheck</t>
   </si>
   <si>
     <t>TotalsWithinToleranceCheck</t>
   </si>
   <si>
-    <t>MultiMatchCheck</t>
-  </si>
-  <si>
     <t>TRANSACTIONS_MATCHED_BETWEEN_SALES_AND_TDSLEDGER</t>
   </si>
   <si>
@@ -196,6 +179,79 @@
   </si>
   <si>
     <t>_26as.taxFiled</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Deposits</t>
+  </si>
+  <si>
+    <t>Withdrawals</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Chequeue #80</t>
+  </si>
+  <si>
+    <t>Cheque #80</t>
+  </si>
+  <si>
+    <t>Chequeue #81</t>
+  </si>
+  <si>
+    <t>Cheque #81</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>sales.invoiceNo</t>
+  </si>
+  <si>
+    <t>tdsLedger.invoiceNo</t>
+  </si>
+  <si>
+    <t>TDS_TOTALS_MATCHED_BETWEEN_SALES_AND_TDSLEDGER</t>
+  </si>
+  <si>
+    <t>TDS_TOTALS_UNMATCHED_BETWEEN_SALES_AND_TDSLEDGER</t>
+  </si>
+  <si>
+    <t>TDS_TOTALS_MATCHED_BETWEEN_TDSLEDGER_AND_26AS</t>
+  </si>
+  <si>
+    <t>TDS_TOTALS_UNMATCHED_BETWEEN_TDSLEDGER_AND_26AS</t>
+  </si>
+  <si>
+    <t>EntryWiseChecks</t>
+  </si>
+  <si>
+    <t>OneToOneChecks</t>
+  </si>
+  <si>
+    <t>sales.invoiceNo == tdsLedger.InvoiceNo AND 
+valueWithinTolerance(sales.tdsOnSales,tdsLedger.tds, 1.0)</t>
   </si>
 </sst>
 </file>
@@ -272,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -294,6 +350,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,15 +679,15 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61.83203125" style="3" bestFit="1" customWidth="1"/>
@@ -686,15 +754,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
@@ -752,12 +820,12 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -768,10 +836,10 @@
         <v>27</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>14</v>
@@ -788,101 +856,89 @@
         <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F20" s="3">
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>15</v>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>44</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -890,11 +946,125 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A79806-79B3-A140-84D1-1525075DFC1E}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="13">
+        <v>44682</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3">
+        <v>468</v>
+      </c>
+      <c r="J3" s="13">
+        <v>44682</v>
+      </c>
+      <c r="K3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
+        <v>44682</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4">
+        <v>390</v>
+      </c>
+      <c r="J4" s="13">
+        <v>44682</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>44682</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="J5" s="13">
+        <v>44682</v>
+      </c>
+      <c r="K5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7D779E-EB07-734E-9825-AAAD9C9C2695}">
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,7 +1084,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -922,7 +1092,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -936,10 +1106,10 @@
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>28</v>
@@ -950,7 +1120,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>29</v>
@@ -961,10 +1131,10 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>10</v>
@@ -1139,7 +1309,7 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>

</xml_diff>